<commit_message>
nuevo stock, corrección catalogo orden
</commit_message>
<xml_diff>
--- a/netlify/functions/Productos.xlsx
+++ b/netlify/functions/Productos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ignacio Aguilera\Desktop\Trabajo (SPA)\IvelPink\netlify\functions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1DAAD43-FEE6-4D85-BA67-4694C6D04D04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED6C3375-B0A7-453A-B83F-92803B61918B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="63">
   <si>
     <t>IdProducto</t>
   </si>
@@ -158,13 +158,64 @@
   </si>
   <si>
     <t>/Producto1.mp4</t>
+  </si>
+  <si>
+    <t>Pijama 19</t>
+  </si>
+  <si>
+    <t>Pijama 20</t>
+  </si>
+  <si>
+    <t>Pijama 21</t>
+  </si>
+  <si>
+    <t>Pijama 22</t>
+  </si>
+  <si>
+    <t>Pijama 23</t>
+  </si>
+  <si>
+    <t>Pijama 24</t>
+  </si>
+  <si>
+    <t>Pijama 25</t>
+  </si>
+  <si>
+    <t>productos/producto-1.webp</t>
+  </si>
+  <si>
+    <t>productos/producto-2.webp</t>
+  </si>
+  <si>
+    <t>productos/producto-3.webp</t>
+  </si>
+  <si>
+    <t>productos/producto-4.webp</t>
+  </si>
+  <si>
+    <t>productos/producto-5.webp</t>
+  </si>
+  <si>
+    <t>productos/producto-6.webp</t>
+  </si>
+  <si>
+    <t>productos/producto-7.webp</t>
+  </si>
+  <si>
+    <t>Orden</t>
+  </si>
+  <si>
+    <t>/productos/producto-1.mp4</t>
+  </si>
+  <si>
+    <t>/productos/producto-2.mp4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -176,6 +227,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -525,15 +582,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -558,8 +623,11 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I1" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -584,8 +652,11 @@
       <c r="H2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -610,8 +681,11 @@
       <c r="H3" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -636,8 +710,11 @@
       <c r="H4" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -662,8 +739,11 @@
       <c r="H5" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I5">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -688,8 +768,11 @@
       <c r="H6" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I6">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -714,8 +797,11 @@
       <c r="H7" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I7">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -740,8 +826,11 @@
       <c r="H8" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -766,8 +855,11 @@
       <c r="H9" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -792,8 +884,11 @@
       <c r="H10" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I10">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -818,8 +913,11 @@
       <c r="H11" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I11">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -844,8 +942,11 @@
       <c r="H12" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I12">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -870,8 +971,11 @@
       <c r="H13" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I13">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -896,8 +1000,11 @@
       <c r="H14" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I14">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -922,8 +1029,11 @@
       <c r="H15" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I15">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -948,8 +1058,11 @@
       <c r="H16" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I16">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -974,8 +1087,11 @@
       <c r="H17" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I17">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1000,8 +1116,11 @@
       <c r="H18" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I18">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1026,8 +1145,215 @@
       <c r="H19" t="s">
         <v>45</v>
       </c>
+      <c r="I19">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20" t="s">
+        <v>26</v>
+      </c>
+      <c r="D20">
+        <v>10000</v>
+      </c>
+      <c r="E20">
+        <v>5</v>
+      </c>
+      <c r="F20" t="s">
+        <v>53</v>
+      </c>
+      <c r="G20" t="b">
+        <v>1</v>
+      </c>
+      <c r="H20" t="s">
+        <v>61</v>
+      </c>
+      <c r="I20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>47</v>
+      </c>
+      <c r="C21" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21">
+        <v>10000</v>
+      </c>
+      <c r="E21">
+        <v>5</v>
+      </c>
+      <c r="F21" t="s">
+        <v>54</v>
+      </c>
+      <c r="G21" t="b">
+        <v>0</v>
+      </c>
+      <c r="H21" t="s">
+        <v>45</v>
+      </c>
+      <c r="I21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>48</v>
+      </c>
+      <c r="C22" t="s">
+        <v>26</v>
+      </c>
+      <c r="D22">
+        <v>6000</v>
+      </c>
+      <c r="E22">
+        <v>5</v>
+      </c>
+      <c r="F22" t="s">
+        <v>55</v>
+      </c>
+      <c r="G22" t="b">
+        <v>0</v>
+      </c>
+      <c r="H22" t="s">
+        <v>62</v>
+      </c>
+      <c r="I22">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23" t="s">
+        <v>26</v>
+      </c>
+      <c r="D23">
+        <v>3000</v>
+      </c>
+      <c r="E23">
+        <v>5</v>
+      </c>
+      <c r="F23" t="s">
+        <v>56</v>
+      </c>
+      <c r="G23" t="b">
+        <v>0</v>
+      </c>
+      <c r="H23" t="s">
+        <v>62</v>
+      </c>
+      <c r="I23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>50</v>
+      </c>
+      <c r="C24" t="s">
+        <v>26</v>
+      </c>
+      <c r="D24">
+        <v>8000</v>
+      </c>
+      <c r="E24">
+        <v>5</v>
+      </c>
+      <c r="F24" t="s">
+        <v>57</v>
+      </c>
+      <c r="G24" t="b">
+        <v>0</v>
+      </c>
+      <c r="H24" t="s">
+        <v>45</v>
+      </c>
+      <c r="I24">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>51</v>
+      </c>
+      <c r="C25" t="s">
+        <v>26</v>
+      </c>
+      <c r="D25">
+        <v>15000</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25" t="s">
+        <v>58</v>
+      </c>
+      <c r="G25" t="b">
+        <v>0</v>
+      </c>
+      <c r="H25" t="s">
+        <v>45</v>
+      </c>
+      <c r="I25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>52</v>
+      </c>
+      <c r="C26" t="s">
+        <v>26</v>
+      </c>
+      <c r="D26">
+        <v>10000</v>
+      </c>
+      <c r="E26">
+        <v>3</v>
+      </c>
+      <c r="F26" t="s">
+        <v>59</v>
+      </c>
+      <c r="G26" t="b">
+        <v>0</v>
+      </c>
+      <c r="H26" t="s">
+        <v>45</v>
+      </c>
+      <c r="I26">
+        <v>7</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>